<commit_message>
added papers, updated tables
</commit_message>
<xml_diff>
--- a/spreadsheets/behavioral.xlsx
+++ b/spreadsheets/behavioral.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Studies" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Eye tracking measures" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Eye_tracking_measures" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Factors" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Model-based estimation of the state of vehicle automation as derived from the driver’s spontaneous visual strategies </t>
+          <t>Model-based estimation of the state of vehicle automation as derived from the driver’s spontaneous visual strategies</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gazing Characteristics of a Driver during Vehicle Backing </t>
+          <t>Gazing Characteristics of a Driver during Vehicle Backing</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3640,7 +3640,7 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve">STISIM </t>
+          <t>STISIM</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
@@ -5784,7 +5784,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t xml:space="preserve">STISIM </t>
+          <t>STISIM</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
@@ -7608,7 +7608,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t xml:space="preserve">custom </t>
+          <t>custom</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -8264,7 +8264,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t xml:space="preserve">28 M, 24 F, mean ages for younger drivers 24 +- 3 and 66 +-2 for older drivers, at least 3 years of driving experience </t>
+          <t>28 M, 24 F, mean ages for younger drivers 24 +- 3 and 66 +-2 for older drivers, at least 3 years of driving experience</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -8793,7 +8793,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t xml:space="preserve">STISIM </t>
+          <t>STISIM</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -9792,7 +9792,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t xml:space="preserve">STISIM </t>
+          <t>STISIM</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -10073,7 +10073,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t xml:space="preserve">25 M, 15 F, equally split between young (mean age 27+-5 years) and older (73+-6 years), driven within past 3 months, with 2+ years of driving experience </t>
+          <t>25 M, 15 F, equally split between young (mean age 27+-5 years) and older (73+-6 years), driven within past 3 months, with 2+ years of driving experience</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
@@ -12090,7 +12090,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t xml:space="preserve">25 M, 15 F, equally split between young (mean age 27+-5 years) and older (73+-6 years), driven within past 3 months, with 2+ years of driving experience </t>
+          <t>25 M, 15 F, equally split between young (mean age 27+-5 years) and older (73+-6 years), driven within past 3 months, with 2+ years of driving experience</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -13165,7 +13165,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t xml:space="preserve">custom </t>
+          <t>custom</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
@@ -13378,7 +13378,7 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t xml:space="preserve">custom </t>
+          <t>custom</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -13765,7 +13765,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t xml:space="preserve">STISIM </t>
+          <t>STISIM</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -15096,7 +15096,7 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t xml:space="preserve">custom </t>
+          <t>custom</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
@@ -15933,7 +15933,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t xml:space="preserve">STISIM </t>
+          <t>STISIM</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -16257,7 +16257,7 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t xml:space="preserve">custom </t>
+          <t>custom</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -17493,7 +17493,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t xml:space="preserve">DriveSafety </t>
+          <t>DriveSafety</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">

</xml_diff>